<commit_message>
up to maternal mortality
</commit_message>
<xml_diff>
--- a/Formatted_Excel_Files/State of the Tropics_Society_Female Education.xlsx
+++ b/Formatted_Excel_Files/State of the Tropics_Society_Female Education.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="17520" windowHeight="13200" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="17520" windowHeight="13200" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tropics" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
     <sheet name="Tropics-Tableau" sheetId="5" r:id="rId4"/>
     <sheet name="Rest of the World-Tableau" sheetId="6" r:id="rId5"/>
+    <sheet name="Summary-Tableau" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3348" uniqueCount="224">
   <si>
     <t>Major area, region, country or area</t>
   </si>
@@ -680,15 +681,6 @@
     <t>New Zealand</t>
   </si>
   <si>
-    <t>SOURCE:</t>
-  </si>
-  <si>
-    <t>Barro and Lee Educational Attainment Dataset</t>
-  </si>
-  <si>
-    <t>http://www.barrolee.com/</t>
-  </si>
-  <si>
     <t>Ratio of Females to males with at least secondary education</t>
   </si>
   <si>
@@ -696,6 +688,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -8669,7 +8664,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8681,50 +8676,184 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>223</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1950</v>
+      </c>
+      <c r="C1" s="5">
+        <v>1960</v>
+      </c>
+      <c r="D1" s="5">
+        <v>1970</v>
+      </c>
+      <c r="E1" s="5">
+        <v>1980</v>
+      </c>
+      <c r="F1" s="5">
+        <v>1990</v>
+      </c>
+      <c r="G1" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H1" s="5">
+        <v>2010</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>118</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.33846432905574281</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.40213326412000522</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.45225999435357039</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.49180666550855706</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.60856787378648602</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.68824396042150227</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.74699367005620931</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.35283115421380457</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.29337322429657381</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.26853792337954385</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.32824825500966393</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.40432962053686489</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.46470542365561007</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.54424545472184283</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.18377202136659837</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.2028752664286039</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.20614220294206151</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.25487397575031395</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.35518935234625959</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.47979024583920038</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.58239969332417518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.17321550612720013</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.20263906331502751</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.27207032910533513</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.33022649190158637</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.42377197273025669</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.51287670559908149</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.56621945117689099</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>56</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.28533558026941408</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.33344592646567989</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.42021934523717602</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.53255638758625301</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.68964526722930841</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.75389196204626208</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.82742480740197044</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>1950</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1960</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1970</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1980</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1990</v>
-      </c>
-      <c r="G7" s="5">
-        <v>2000</v>
-      </c>
-      <c r="H7" s="5">
-        <v>2010</v>
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.75001985696727025</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.78198384644787355</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.76634188950909499</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.80614254820792886</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.84019566226728482</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.91365605113922366</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.94453742084953829</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -8753,28 +8882,28 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B8" s="6">
-        <v>0.33846432905574281</v>
+        <v>0.72267166431848262</v>
       </c>
       <c r="C8" s="6">
-        <v>0.40213326412000522</v>
+        <v>0.74846287255983135</v>
       </c>
       <c r="D8" s="6">
-        <v>0.45225999435357039</v>
+        <v>0.79278325088768964</v>
       </c>
       <c r="E8" s="6">
-        <v>0.49180666550855706</v>
+        <v>0.72381016211128268</v>
       </c>
       <c r="F8" s="6">
-        <v>0.60856787378648602</v>
+        <v>0.83992098666563231</v>
       </c>
       <c r="G8" s="6">
-        <v>0.68824396042150227</v>
+        <v>0.87293997435582427</v>
       </c>
       <c r="H8" s="6">
-        <v>0.74699367005620931</v>
+        <v>0.89513158119402714</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -8803,28 +8932,28 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="B9" s="6">
-        <v>0.35283115421380457</v>
+        <v>0.65691817844342926</v>
       </c>
       <c r="C9" s="6">
-        <v>0.29337322429657381</v>
+        <v>0.7044339641695917</v>
       </c>
       <c r="D9" s="6">
-        <v>0.26853792337954385</v>
+        <v>0.76053247389632039</v>
       </c>
       <c r="E9" s="6">
-        <v>0.32824825500966393</v>
+        <v>0.84264106440443287</v>
       </c>
       <c r="F9" s="6">
-        <v>0.40432962053686489</v>
+        <v>0.96458073575534431</v>
       </c>
       <c r="G9" s="6">
-        <v>0.46470542365561007</v>
+        <v>1.0013847406309961</v>
       </c>
       <c r="H9" s="6">
-        <v>0.54424545472184283</v>
+        <v>0.99441822288484738</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -8853,28 +8982,28 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="B10" s="6">
-        <v>0.18377202136659837</v>
+        <v>1.0574922921273457</v>
       </c>
       <c r="C10" s="6">
-        <v>0.2028752664286039</v>
+        <v>1.017238532602297</v>
       </c>
       <c r="D10" s="6">
-        <v>0.20614220294206151</v>
+        <v>0.97411819046735837</v>
       </c>
       <c r="E10" s="6">
-        <v>0.25487397575031395</v>
+        <v>0.9776436830148485</v>
       </c>
       <c r="F10" s="6">
-        <v>0.35518935234625959</v>
+        <v>1.0545899621502421</v>
       </c>
       <c r="G10" s="6">
-        <v>0.47979024583920038</v>
+        <v>0.94717717521427736</v>
       </c>
       <c r="H10" s="6">
-        <v>0.58239969332417518</v>
+        <v>0.94757120977120968</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -8903,28 +9032,28 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="B11" s="6">
-        <v>0.17321550612720013</v>
+        <v>0.78703090403713383</v>
       </c>
       <c r="C11" s="6">
-        <v>0.20263906331502751</v>
+        <v>0.80723593373819202</v>
       </c>
       <c r="D11" s="6">
-        <v>0.27207032910533513</v>
+        <v>0.77397113439760901</v>
       </c>
       <c r="E11" s="6">
-        <v>0.33022649190158637</v>
+        <v>0.76942541024669209</v>
       </c>
       <c r="F11" s="6">
-        <v>0.42377197273025669</v>
+        <v>0.84575655359436952</v>
       </c>
       <c r="G11" s="6">
-        <v>0.51287670559908149</v>
+        <v>0.82854251248082322</v>
       </c>
       <c r="H11" s="6">
-        <v>0.56621945117689099</v>
+        <v>0.85522608499211683</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -8953,28 +9082,28 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="B12" s="6">
-        <v>0.28533558026941408</v>
+        <v>0.750056417272565</v>
       </c>
       <c r="C12" s="6">
-        <v>0.33344592646567989</v>
+        <v>0.77734128427029203</v>
       </c>
       <c r="D12" s="6">
-        <v>0.42021934523717602</v>
+        <v>0.74109560115877116</v>
       </c>
       <c r="E12" s="6">
-        <v>0.53255638758625301</v>
+        <v>0.72637284248556833</v>
       </c>
       <c r="F12" s="6">
-        <v>0.68964526722930841</v>
+        <v>0.80084614237562379</v>
       </c>
       <c r="G12" s="6">
-        <v>0.75389196204626208</v>
+        <v>0.79955621951283107</v>
       </c>
       <c r="H12" s="6">
-        <v>0.82742480740197044</v>
+        <v>0.82919815484480974</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -9002,30 +9131,6 @@
       <c r="AF12" s="4"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.75001985696727025</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.78198384644787355</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.76634188950909499</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.80614254820792886</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.84019566226728482</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.91365605113922366</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0.94453742084953829</v>
-      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -9052,30 +9157,6 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.72267166431848262</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.74846287255983135</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0.79278325088768964</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0.72381016211128268</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.83992098666563231</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0.87293997435582427</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.89513158119402714</v>
-      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -9102,30 +9183,6 @@
       <c r="AF14" s="4"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.65691817844342926</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.7044339641695917</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0.76053247389632039</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.84264106440443287</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.96458073575534431</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1.0013847406309961</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0.99441822288484738</v>
-      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -9152,30 +9209,6 @@
       <c r="AF15" s="4"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1.0574922921273457</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1.017238532602297</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0.97411819046735837</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.9776436830148485</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1.0545899621502421</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0.94717717521427736</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0.94757120977120968</v>
-      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -9201,31 +9234,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0.78703090403713383</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.80723593373819202</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0.77397113439760901</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.76942541024669209</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0.84575655359436952</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0.82854251248082322</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0.85522608499211683</v>
-      </c>
+    <row r="17" spans="9:32" x14ac:dyDescent="0.25">
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -9251,31 +9260,7 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="6">
-        <v>0.750056417272565</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0.77734128427029203</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.74109560115877116</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.72637284248556833</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0.80084614237562379</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0.79955621951283107</v>
-      </c>
-      <c r="H18" s="6">
-        <v>0.82919815484480974</v>
-      </c>
+    <row r="18" spans="9:32" x14ac:dyDescent="0.25">
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -9329,10 +9314,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -22616,8 +22601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1003" sqref="A1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22631,10 +22616,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -33932,6 +33917,879 @@
       </c>
       <c r="C1028">
         <v>0.97676904893441352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2">
+        <v>1950</v>
+      </c>
+      <c r="C2">
+        <v>0.33846432905574281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3">
+        <v>1960</v>
+      </c>
+      <c r="C3">
+        <v>0.40213326412000522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4">
+        <v>1970</v>
+      </c>
+      <c r="C4">
+        <v>0.45225999435357039</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>1980</v>
+      </c>
+      <c r="C5">
+        <v>0.49180666550855706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6">
+        <v>1990</v>
+      </c>
+      <c r="C6">
+        <v>0.60856787378648602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <v>0.68824396042150227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8">
+        <v>2010</v>
+      </c>
+      <c r="C8">
+        <v>0.74699367005620931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1950</v>
+      </c>
+      <c r="C9">
+        <v>0.35283115421380457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1960</v>
+      </c>
+      <c r="C10">
+        <v>0.29337322429657381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1970</v>
+      </c>
+      <c r="C11">
+        <v>0.26853792337954385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1980</v>
+      </c>
+      <c r="C12">
+        <v>0.32824825500966393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1990</v>
+      </c>
+      <c r="C13">
+        <v>0.40432962053686489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>2000</v>
+      </c>
+      <c r="C14">
+        <v>0.46470542365561007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>2010</v>
+      </c>
+      <c r="C15">
+        <v>0.54424545472184283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>1950</v>
+      </c>
+      <c r="C16">
+        <v>0.18377202136659837</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>1960</v>
+      </c>
+      <c r="C17">
+        <v>0.2028752664286039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>1970</v>
+      </c>
+      <c r="C18">
+        <v>0.20614220294206151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>1980</v>
+      </c>
+      <c r="C19">
+        <v>0.25487397575031395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>1990</v>
+      </c>
+      <c r="C20">
+        <v>0.35518935234625959</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>2000</v>
+      </c>
+      <c r="C21">
+        <v>0.47979024583920038</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>2010</v>
+      </c>
+      <c r="C22">
+        <v>0.58239969332417518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>1950</v>
+      </c>
+      <c r="C23">
+        <v>0.17321550612720013</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24">
+        <v>1960</v>
+      </c>
+      <c r="C24">
+        <v>0.20263906331502751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25">
+        <v>1970</v>
+      </c>
+      <c r="C25">
+        <v>0.27207032910533513</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26">
+        <v>1980</v>
+      </c>
+      <c r="C26">
+        <v>0.33022649190158637</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>1990</v>
+      </c>
+      <c r="C27">
+        <v>0.42377197273025669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28">
+        <v>2000</v>
+      </c>
+      <c r="C28">
+        <v>0.51287670559908149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>2010</v>
+      </c>
+      <c r="C29">
+        <v>0.56621945117689099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30">
+        <v>1950</v>
+      </c>
+      <c r="C30">
+        <v>0.28533558026941408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31">
+        <v>1960</v>
+      </c>
+      <c r="C31">
+        <v>0.33344592646567989</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>1970</v>
+      </c>
+      <c r="C32">
+        <v>0.42021934523717602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33">
+        <v>1980</v>
+      </c>
+      <c r="C33">
+        <v>0.53255638758625301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34">
+        <v>1990</v>
+      </c>
+      <c r="C34">
+        <v>0.68964526722930841</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35">
+        <v>2000</v>
+      </c>
+      <c r="C35">
+        <v>0.75389196204626208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <v>2010</v>
+      </c>
+      <c r="C36">
+        <v>0.82742480740197044</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>1950</v>
+      </c>
+      <c r="C37">
+        <v>0.75001985696727025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>1960</v>
+      </c>
+      <c r="C38">
+        <v>0.78198384644787355</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39">
+        <v>1970</v>
+      </c>
+      <c r="C39">
+        <v>0.76634188950909499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40">
+        <v>1980</v>
+      </c>
+      <c r="C40">
+        <v>0.80614254820792886</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41">
+        <v>1990</v>
+      </c>
+      <c r="C41">
+        <v>0.84019566226728482</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42">
+        <v>2000</v>
+      </c>
+      <c r="C42">
+        <v>0.91365605113922366</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43">
+        <v>2010</v>
+      </c>
+      <c r="C43">
+        <v>0.94453742084953829</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44">
+        <v>1950</v>
+      </c>
+      <c r="C44">
+        <v>0.72267166431848262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45">
+        <v>1960</v>
+      </c>
+      <c r="C45">
+        <v>0.74846287255983135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46">
+        <v>1970</v>
+      </c>
+      <c r="C46">
+        <v>0.79278325088768964</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47">
+        <v>1980</v>
+      </c>
+      <c r="C47">
+        <v>0.72381016211128268</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48">
+        <v>1990</v>
+      </c>
+      <c r="C48">
+        <v>0.83992098666563231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49">
+        <v>2000</v>
+      </c>
+      <c r="C49">
+        <v>0.87293997435582427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50">
+        <v>2010</v>
+      </c>
+      <c r="C50">
+        <v>0.89513158119402714</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51">
+        <v>1950</v>
+      </c>
+      <c r="C51">
+        <v>0.65691817844342926</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52">
+        <v>1960</v>
+      </c>
+      <c r="C52">
+        <v>0.7044339641695917</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53">
+        <v>1970</v>
+      </c>
+      <c r="C53">
+        <v>0.76053247389632039</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54">
+        <v>1980</v>
+      </c>
+      <c r="C54">
+        <v>0.84264106440443287</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55">
+        <v>1990</v>
+      </c>
+      <c r="C55">
+        <v>0.96458073575534431</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56">
+        <v>2000</v>
+      </c>
+      <c r="C56">
+        <v>1.0013847406309961</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57">
+        <v>2010</v>
+      </c>
+      <c r="C57">
+        <v>0.99441822288484738</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58">
+        <v>1950</v>
+      </c>
+      <c r="C58">
+        <v>1.0574922921273457</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59">
+        <v>1960</v>
+      </c>
+      <c r="C59">
+        <v>1.017238532602297</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60">
+        <v>1970</v>
+      </c>
+      <c r="C60">
+        <v>0.97411819046735837</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61">
+        <v>1980</v>
+      </c>
+      <c r="C61">
+        <v>0.9776436830148485</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62">
+        <v>1990</v>
+      </c>
+      <c r="C62">
+        <v>1.0545899621502421</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63">
+        <v>2000</v>
+      </c>
+      <c r="C63">
+        <v>0.94717717521427736</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64">
+        <v>2010</v>
+      </c>
+      <c r="C64">
+        <v>0.94757120977120968</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65">
+        <v>1950</v>
+      </c>
+      <c r="C65">
+        <v>0.78703090403713383</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66">
+        <v>1960</v>
+      </c>
+      <c r="C66">
+        <v>0.80723593373819202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67">
+        <v>1970</v>
+      </c>
+      <c r="C67">
+        <v>0.77397113439760901</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68">
+        <v>1980</v>
+      </c>
+      <c r="C68">
+        <v>0.76942541024669209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69">
+        <v>1990</v>
+      </c>
+      <c r="C69">
+        <v>0.84575655359436952</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70">
+        <v>2000</v>
+      </c>
+      <c r="C70">
+        <v>0.82854251248082322</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71">
+        <v>2010</v>
+      </c>
+      <c r="C71">
+        <v>0.85522608499211683</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1950</v>
+      </c>
+      <c r="C72">
+        <v>0.750056417272565</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1960</v>
+      </c>
+      <c r="C73">
+        <v>0.77734128427029203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>1970</v>
+      </c>
+      <c r="C74">
+        <v>0.74109560115877116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>1980</v>
+      </c>
+      <c r="C75">
+        <v>0.72637284248556833</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>1990</v>
+      </c>
+      <c r="C76">
+        <v>0.80084614237562379</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>2000</v>
+      </c>
+      <c r="C77">
+        <v>0.79955621951283107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>2010</v>
+      </c>
+      <c r="C78">
+        <v>0.82919815484480974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>